<commit_message>
dead end lot values and a13 adaptation
</commit_message>
<xml_diff>
--- a/management/TODO.xlsx
+++ b/management/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>卢冰</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>郑永祥</t>
+  </si>
+  <si>
+    <t>茅勤</t>
+  </si>
+  <si>
+    <t>朱保全</t>
+  </si>
+  <si>
+    <t>曹京明</t>
+  </si>
+  <si>
+    <t>吴轶秦</t>
+  </si>
+  <si>
+    <t>郭散皞</t>
+  </si>
+  <si>
+    <t>领导，之前跟您汇报过一次，我开发了一个辅助车位定价的系统，现在可以运转。</t>
+  </si>
+  <si>
+    <t>我是北京区域设计部的李谦，曾经跟您见过几面。我最近研发了一个服务于车位定价的系统。这个系统对咱们现在的工作可能有一些价值。冒昧给您发一些资料，争取一些您的关注。这个系统采用了一些技术手段，可以给项目提供精细的车位定价方案。可以作为管理抓手、提高定价方案的质量、节约管理人力、提高透明度；解决车位销售中管理难度大、价值流失和透明度不足导致的客户信任问题。推荐给您是我考虑这个系统可能需要比较大的体量以产生足够价值。我给您附上一个介绍，期待您的指导和建议。</t>
   </si>
 </sst>
 </file>
@@ -207,13 +228,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,11 +521,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="85" style="5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -538,15 +565,18 @@
         <v>3</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1"/>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -572,67 +602,70 @@
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -651,6 +684,33 @@
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>